<commit_message>
Kakao Map shows Green and Yellow Circle Markers
The webpage now differentiates between Green (LCD) and Yellow (QR) Stations and update them with green and yellow circle markers respectively on Kakao Map.
</commit_message>
<xml_diff>
--- a/서울특별시 공공자전거 데이터/서울특별시 공공자전거 대여소 정보(19.12.9).xlsx
+++ b/서울특별시 공공자전거 데이터/서울특별시 공공자전거 대여소 정보(19.12.9).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vandy_Drive\Github\randy-seoul-bike\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vandy_Drive\Github\randy-seoul-bike\서울특별시 공공자전거 데이터\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206D443E-E116-4E48-A46E-ED28778B72F1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA38897-6A84-4B92-9BF5-27B5BB1F5209}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="507" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11535,7 +11535,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$2" spid="_x0000_s40373"/>
+                  <a14:cameraTool cellRange="$D$2" spid="_x0000_s40423"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -11601,7 +11601,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$3" spid="_x0000_s40374"/>
+                  <a14:cameraTool cellRange="$D$3" spid="_x0000_s40424"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -11667,7 +11667,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$4" spid="_x0000_s40375"/>
+                  <a14:cameraTool cellRange="$D$4" spid="_x0000_s40425"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -11733,7 +11733,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$5" spid="_x0000_s40376"/>
+                  <a14:cameraTool cellRange="$D$5" spid="_x0000_s40426"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -11799,7 +11799,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$6" spid="_x0000_s40377"/>
+                  <a14:cameraTool cellRange="$D$6" spid="_x0000_s40427"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -11865,7 +11865,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$7" spid="_x0000_s40378"/>
+                  <a14:cameraTool cellRange="$D$7" spid="_x0000_s40428"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -11931,7 +11931,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$8" spid="_x0000_s40379"/>
+                  <a14:cameraTool cellRange="$D$8" spid="_x0000_s40429"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -11997,7 +11997,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$9" spid="_x0000_s40380"/>
+                  <a14:cameraTool cellRange="$D$9" spid="_x0000_s40430"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12063,7 +12063,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$10" spid="_x0000_s40381"/>
+                  <a14:cameraTool cellRange="$D$10" spid="_x0000_s40431"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12129,7 +12129,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$11" spid="_x0000_s40382"/>
+                  <a14:cameraTool cellRange="$D$11" spid="_x0000_s40432"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12195,7 +12195,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$12" spid="_x0000_s40383"/>
+                  <a14:cameraTool cellRange="$D$12" spid="_x0000_s40433"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12261,7 +12261,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$13" spid="_x0000_s40384"/>
+                  <a14:cameraTool cellRange="$D$13" spid="_x0000_s40434"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12327,7 +12327,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$14" spid="_x0000_s40385"/>
+                  <a14:cameraTool cellRange="$D$14" spid="_x0000_s40435"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12393,7 +12393,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$15" spid="_x0000_s40386"/>
+                  <a14:cameraTool cellRange="$D$15" spid="_x0000_s40436"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12459,7 +12459,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$16" spid="_x0000_s40387"/>
+                  <a14:cameraTool cellRange="$D$16" spid="_x0000_s40437"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12525,7 +12525,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$17" spid="_x0000_s40388"/>
+                  <a14:cameraTool cellRange="$D$17" spid="_x0000_s40438"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12591,7 +12591,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$18" spid="_x0000_s40389"/>
+                  <a14:cameraTool cellRange="$D$18" spid="_x0000_s40439"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12657,7 +12657,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$20" spid="_x0000_s40390"/>
+                  <a14:cameraTool cellRange="$D$20" spid="_x0000_s40440"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12723,7 +12723,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$21" spid="_x0000_s40391"/>
+                  <a14:cameraTool cellRange="$D$21" spid="_x0000_s40441"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12789,7 +12789,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$22" spid="_x0000_s40392"/>
+                  <a14:cameraTool cellRange="$D$22" spid="_x0000_s40442"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12855,7 +12855,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$23" spid="_x0000_s40393"/>
+                  <a14:cameraTool cellRange="$D$23" spid="_x0000_s40443"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12921,7 +12921,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$24" spid="_x0000_s40394"/>
+                  <a14:cameraTool cellRange="$D$24" spid="_x0000_s40444"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -12987,7 +12987,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$25" spid="_x0000_s40395"/>
+                  <a14:cameraTool cellRange="$D$25" spid="_x0000_s40445"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13053,7 +13053,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$26" spid="_x0000_s40396"/>
+                  <a14:cameraTool cellRange="$D$26" spid="_x0000_s40446"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13119,7 +13119,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$D$19" spid="_x0000_s40397"/>
+                  <a14:cameraTool cellRange="$D$19" spid="_x0000_s40447"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13185,7 +13185,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$2" spid="_x0000_s40398"/>
+                  <a14:cameraTool cellRange="$C$2" spid="_x0000_s40448"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13251,7 +13251,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$3" spid="_x0000_s40399"/>
+                  <a14:cameraTool cellRange="$C$3" spid="_x0000_s40449"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13317,7 +13317,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$4" spid="_x0000_s40400"/>
+                  <a14:cameraTool cellRange="$C$4" spid="_x0000_s40450"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13383,7 +13383,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$5" spid="_x0000_s40401"/>
+                  <a14:cameraTool cellRange="$C$5" spid="_x0000_s40451"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13449,7 +13449,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$6" spid="_x0000_s40402"/>
+                  <a14:cameraTool cellRange="$C$6" spid="_x0000_s40452"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13515,7 +13515,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$7" spid="_x0000_s40403"/>
+                  <a14:cameraTool cellRange="$C$7" spid="_x0000_s40453"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13581,7 +13581,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$8" spid="_x0000_s40404"/>
+                  <a14:cameraTool cellRange="$C$8" spid="_x0000_s40454"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13647,7 +13647,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$9" spid="_x0000_s40405"/>
+                  <a14:cameraTool cellRange="$C$9" spid="_x0000_s40455"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13713,7 +13713,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$10" spid="_x0000_s40406"/>
+                  <a14:cameraTool cellRange="$C$10" spid="_x0000_s40456"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13779,7 +13779,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$11" spid="_x0000_s40407"/>
+                  <a14:cameraTool cellRange="$C$11" spid="_x0000_s40457"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13845,7 +13845,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$12" spid="_x0000_s40408"/>
+                  <a14:cameraTool cellRange="$C$12" spid="_x0000_s40458"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13911,7 +13911,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$13" spid="_x0000_s40409"/>
+                  <a14:cameraTool cellRange="$C$13" spid="_x0000_s40459"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13977,7 +13977,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$14" spid="_x0000_s40410"/>
+                  <a14:cameraTool cellRange="$C$14" spid="_x0000_s40460"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14043,7 +14043,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$15" spid="_x0000_s40411"/>
+                  <a14:cameraTool cellRange="$C$15" spid="_x0000_s40461"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14109,7 +14109,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$16" spid="_x0000_s40412"/>
+                  <a14:cameraTool cellRange="$C$16" spid="_x0000_s40462"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14175,7 +14175,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$17" spid="_x0000_s40413"/>
+                  <a14:cameraTool cellRange="$C$17" spid="_x0000_s40463"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14241,7 +14241,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$18" spid="_x0000_s40414"/>
+                  <a14:cameraTool cellRange="$C$18" spid="_x0000_s40464"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14307,7 +14307,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$19" spid="_x0000_s40415"/>
+                  <a14:cameraTool cellRange="$C$19" spid="_x0000_s40465"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14373,7 +14373,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$20" spid="_x0000_s40416"/>
+                  <a14:cameraTool cellRange="$C$20" spid="_x0000_s40466"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14439,7 +14439,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$21" spid="_x0000_s40417"/>
+                  <a14:cameraTool cellRange="$C$21" spid="_x0000_s40467"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14505,7 +14505,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$22" spid="_x0000_s40418"/>
+                  <a14:cameraTool cellRange="$C$22" spid="_x0000_s40468"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14571,7 +14571,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$23" spid="_x0000_s40419"/>
+                  <a14:cameraTool cellRange="$C$23" spid="_x0000_s40469"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14637,7 +14637,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$24" spid="_x0000_s40420"/>
+                  <a14:cameraTool cellRange="$C$24" spid="_x0000_s40470"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14703,7 +14703,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$25" spid="_x0000_s40421"/>
+                  <a14:cameraTool cellRange="$C$25" spid="_x0000_s40471"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14769,7 +14769,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$C$26" spid="_x0000_s40422"/>
+                  <a14:cameraTool cellRange="$C$26" spid="_x0000_s40472"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -15077,7 +15077,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>